<commit_message>
Add benchmarking and refactor group creation logic
Introduces benchmark_both.py for comparative benchmarking between exhaustive and heuristic group assignment methods. Refactors and improves group creation logic in code/creer_groupes.py, adds a more robust Excel loader, and implements a greedy group assignment function. Adds new input and reference files, including code_base and code_refactoring directories with supporting scripts and data. Updates students.py and grouping.py to simplify and clarify group and partition logic. This update also includes new scripts and modules for refactored group assignment and CLI usage.
</commit_message>
<xml_diff>
--- a/code/Groupes SAÉ S3 -constitution.xlsx
+++ b/code/Groupes SAÉ S3 -constitution.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chanouha\Downloads\affectation-groupe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Groupe_QualAlgo\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD50C1E5-05D5-4643-9DED-7C19878A3C96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1275" yWindow="1620" windowWidth="26460" windowHeight="13860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11256" windowHeight="7728" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Liste S3" sheetId="1" r:id="rId1"/>
@@ -19,7 +18,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Liste S3'!$A$1:$AME$47</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase" localSheetId="0">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentManualCount="12"/>
+  <calcPr calcId="152511" concurrentManualCount="12"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -213,7 +212,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -700,28 +699,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AME47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:F47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" customWidth="1"/>
-    <col min="4" max="4" width="15" style="3" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" style="3" customWidth="1"/>
-    <col min="7" max="244" width="11.42578125" style="3" customWidth="1"/>
-    <col min="245" max="1011" width="11.42578125" customWidth="1"/>
-    <col min="1012" max="1020" width="11.5703125"/>
+    <col min="1" max="1" width="23.44140625" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" customWidth="1"/>
+    <col min="4" max="4" width="35.5546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="8.109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" style="3" customWidth="1"/>
+    <col min="7" max="244" width="11.44140625" style="3" customWidth="1"/>
+    <col min="245" max="1011" width="11.44140625" customWidth="1"/>
+    <col min="1012" max="1020" width="11.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1019" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1019" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>9</v>
       </c>
@@ -983,7 +982,7 @@
       <c r="AMD1"/>
       <c r="AME1"/>
     </row>
-    <row r="2" spans="1:1019" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1019" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1001,7 +1000,7 @@
       </c>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:1019" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1019" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1019,7 +1018,7 @@
       </c>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:1019" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1019" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -1040,7 +1039,7 @@
       </c>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:1019" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1019" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -1058,7 +1057,7 @@
       </c>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:1019" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1019" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -1073,7 +1072,7 @@
       </c>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:1019" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1019" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -1094,7 +1093,7 @@
       </c>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:1019" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1019" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1109,7 +1108,7 @@
       </c>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:1019" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1019" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1127,7 +1126,7 @@
       </c>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:1019" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1019" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1142,7 +1141,7 @@
       </c>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:1019" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1019" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1160,7 +1159,7 @@
       </c>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:1019" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1019" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1178,7 +1177,7 @@
       </c>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:1019" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1019" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1196,7 +1195,7 @@
       </c>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:1019" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1019" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1211,7 +1210,7 @@
       </c>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:1019" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1019" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1232,7 +1231,7 @@
       </c>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:1019" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1019" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -1250,7 +1249,7 @@
       </c>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -1265,7 +1264,7 @@
       </c>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -1280,7 +1279,7 @@
       </c>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -1298,7 +1297,7 @@
       </c>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -1316,7 +1315,7 @@
       </c>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -1331,7 +1330,7 @@
       </c>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>46</v>
       </c>
@@ -1349,7 +1348,7 @@
       </c>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>47</v>
       </c>
@@ -1364,7 +1363,7 @@
       </c>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -1385,7 +1384,7 @@
       </c>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -1400,7 +1399,7 @@
       </c>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -1415,7 +1414,7 @@
       </c>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -1430,7 +1429,7 @@
       </c>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -1448,7 +1447,7 @@
       </c>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -1466,7 +1465,7 @@
       </c>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>19</v>
       </c>
@@ -1481,7 +1480,7 @@
       </c>
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>23</v>
       </c>
@@ -1502,7 +1501,7 @@
       </c>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>24</v>
       </c>
@@ -1517,7 +1516,7 @@
       </c>
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>26</v>
       </c>
@@ -1535,7 +1534,7 @@
       </c>
       <c r="G33" s="2"/>
     </row>
-    <row r="34" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>29</v>
       </c>
@@ -1553,7 +1552,7 @@
       </c>
       <c r="G34" s="2"/>
     </row>
-    <row r="35" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>30</v>
       </c>
@@ -1568,7 +1567,7 @@
       </c>
       <c r="G35" s="2"/>
     </row>
-    <row r="36" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -1583,7 +1582,7 @@
       </c>
       <c r="G36" s="2"/>
     </row>
-    <row r="37" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -1601,7 +1600,7 @@
       </c>
       <c r="G37" s="2"/>
     </row>
-    <row r="38" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>40</v>
       </c>
@@ -1616,7 +1615,7 @@
       </c>
       <c r="G38" s="2"/>
     </row>
-    <row r="39" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>41</v>
       </c>
@@ -1634,7 +1633,7 @@
       </c>
       <c r="G39" s="2"/>
     </row>
-    <row r="40" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>44</v>
       </c>
@@ -1652,7 +1651,7 @@
       </c>
       <c r="G40" s="2"/>
     </row>
-    <row r="41" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -1670,7 +1669,7 @@
       </c>
       <c r="G41" s="2"/>
     </row>
-    <row r="42" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>48</v>
       </c>
@@ -1688,7 +1687,7 @@
       </c>
       <c r="G42" s="2"/>
     </row>
-    <row r="43" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>49</v>
       </c>
@@ -1703,7 +1702,7 @@
       </c>
       <c r="G43" s="2"/>
     </row>
-    <row r="44" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>50</v>
       </c>
@@ -1718,7 +1717,7 @@
       </c>
       <c r="G44" s="2"/>
     </row>
-    <row r="45" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>52</v>
       </c>
@@ -1736,7 +1735,7 @@
       </c>
       <c r="G45" s="2"/>
     </row>
-    <row r="46" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>53</v>
       </c>
@@ -1751,7 +1750,7 @@
       </c>
       <c r="G46" s="2"/>
     </row>
-    <row r="47" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>55</v>
       </c>
@@ -1767,8 +1766,8 @@
       <c r="G47" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AME47" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AME47">
+  <autoFilter ref="A1:AME47">
+    <sortState ref="A2:AME47">
       <sortCondition ref="C1:C47"/>
     </sortState>
   </autoFilter>

</xml_diff>